<commit_message>
Functioneel ontwerp, Planning, Cleanup directory
</commit_message>
<xml_diff>
--- a/Documenten/PLANNING.xlsx
+++ b/Documenten/PLANNING.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>Planning</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>* mondeling besproken (komt terug in FO)</t>
+  </si>
+  <si>
+    <t>* 14.10 - 14.25</t>
   </si>
 </sst>
 </file>
@@ -740,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>65</v>
@@ -1033,7 +1036,7 @@
         <v>43</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1207,7 +1210,7 @@
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
-        <v>41717</v>
+        <v>41724</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>8</v>
@@ -1220,6 +1223,9 @@
       </c>
       <c r="E31" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>